<commit_message>
caes from New FVA Job Type
</commit_message>
<xml_diff>
--- a/TestData/TMTI0056880_ValidateNewJobTypesAvailability.xlsx
+++ b/TestData/TMTI0056880_ValidateNewJobTypesAvailability.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay.kumar\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VKumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDAA41B-02A0-44FD-A447-47DBB7281107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81BB5A0-5530-44BB-AE12-3CD764B00F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -814,13 +814,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -828,7 +828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -846,20 +846,20 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
@@ -879,65 +879,65 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>

</xml_diff>